<commit_message>
multi var mean graph added
</commit_message>
<xml_diff>
--- a/templates/updated secondary figures_060622.xlsx
+++ b/templates/updated secondary figures_060622.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HBSC project\hbsc_compile_report\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71B02F3-718E-4CEC-B2D9-3C821D0422B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C3AF86-F430-4E07-B166-860647B4F6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="secondary figures" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="213">
   <si>
     <t>Figure</t>
   </si>
@@ -653,6 +653,12 @@
   </si>
   <si>
     <t>EMC_Problem</t>
+  </si>
+  <si>
+    <t>Outstanding</t>
+  </si>
+  <si>
+    <t>What does high/poor quality mean numbers-wise?</t>
   </si>
 </sst>
 </file>
@@ -1608,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +1628,7 @@
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1638,14 +1644,17 @@
       <c r="E1" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" s="9" t="s">
         <v>195</v>
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1662,7 +1671,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1679,7 +1688,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1696,7 +1705,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1713,7 +1722,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1730,7 +1739,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1746,8 +1755,11 @@
       <c r="E8" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1764,7 +1776,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1781,7 +1793,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1798,7 +1810,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1815,7 +1827,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1832,7 +1844,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1849,7 +1861,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1866,7 +1878,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
temp function for testing whether combine all gender/grade multivars
</commit_message>
<xml_diff>
--- a/templates/updated secondary figures_060622.xlsx
+++ b/templates/updated secondary figures_060622.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HBSC project\hbsc_compile_report\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C3AF86-F430-4E07-B166-860647B4F6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D49B3A3-BCF9-40E1-A3AA-3A5061759840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="secondary figures" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="215">
   <si>
     <t>Figure</t>
   </si>
@@ -208,9 +208,6 @@
     <t>Figure 31</t>
   </si>
   <si>
-    <t>% pupils who reported substance use in their lifetime</t>
-  </si>
-  <si>
     <t>Figure 32</t>
   </si>
   <si>
@@ -659,6 +656,15 @@
   </si>
   <si>
     <t>What does high/poor quality mean numbers-wise?</t>
+  </si>
+  <si>
+    <t>Figure 31a</t>
+  </si>
+  <si>
+    <t>% pupils who reported substance use in their lifetime, by gender</t>
+  </si>
+  <si>
+    <t>% pupils who reported substance use in their lifetime, by school year</t>
   </si>
 </sst>
 </file>
@@ -1614,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,21 +1642,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -1662,13 +1668,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,13 +1685,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1696,13 +1702,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1713,13 +1719,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1730,13 +1736,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,16 +1753,16 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1767,13 +1773,13 @@
         <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" t="s">
         <v>155</v>
-      </c>
-      <c r="E9" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1784,13 +1790,13 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1801,13 +1807,13 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1818,13 +1824,13 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1835,13 +1841,13 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1852,13 +1858,13 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1869,13 +1875,13 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1886,13 +1892,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1903,13 +1909,13 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1920,13 +1926,13 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1937,13 +1943,13 @@
         <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1954,13 +1960,13 @@
         <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1971,13 +1977,13 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1988,13 +1994,13 @@
         <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2005,13 +2011,13 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2022,13 +2028,13 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2039,13 +2045,13 @@
         <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2056,13 +2062,13 @@
         <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2073,13 +2079,13 @@
         <v>49</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2090,13 +2096,13 @@
         <v>52</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2107,13 +2113,13 @@
         <v>54</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2124,13 +2130,13 @@
         <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2141,16 +2147,16 @@
         <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -2158,13 +2164,13 @@
         <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2172,417 +2178,434 @@
         <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" t="s">
-        <v>99</v>
+        <v>213</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E33" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>212</v>
+      </c>
+      <c r="B34" t="s">
+        <v>214</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" t="s">
-        <v>172</v>
+      <c r="E34" s="7" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" t="s">
         <v>65</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>66</v>
       </c>
-      <c r="C35" t="s">
-        <v>98</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="B37" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" t="s">
         <v>142</v>
-      </c>
-      <c r="E35" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" t="s">
-        <v>176</v>
-      </c>
-      <c r="C36" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" t="s">
-        <v>151</v>
       </c>
       <c r="E37" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" t="s">
+        <v>150</v>
+      </c>
+      <c r="E38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" t="s">
+        <v>150</v>
+      </c>
+      <c r="E39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>70</v>
       </c>
-      <c r="B38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" t="s">
-        <v>151</v>
-      </c>
-      <c r="E38" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B40" t="s">
         <v>71</v>
       </c>
-      <c r="B39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" t="s">
-        <v>137</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>109</v>
+      <c r="C40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" t="s">
-        <v>127</v>
-      </c>
-      <c r="C44" t="s">
-        <v>98</v>
-      </c>
-      <c r="D44" t="s">
-        <v>125</v>
-      </c>
-      <c r="E44" t="s">
-        <v>181</v>
+      <c r="C44" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D45" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D46" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E46" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="E48" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D49" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="E49" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D50" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E50" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" t="s">
+        <v>97</v>
+      </c>
+      <c r="D52" t="s">
+        <v>138</v>
+      </c>
+      <c r="E52" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" t="s">
         <v>95</v>
       </c>
-      <c r="B52" t="s">
-        <v>96</v>
-      </c>
-      <c r="C52" t="s">
-        <v>98</v>
-      </c>
-      <c r="D52" t="s">
-        <v>140</v>
-      </c>
-      <c r="E52" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="C53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" t="s">
+        <v>139</v>
+      </c>
+      <c r="E53" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>195</v>
+      </c>
+      <c r="C56" t="s">
         <v>196</v>
       </c>
-      <c r="C55" t="s">
+      <c r="E56" t="s">
         <v>197</v>
-      </c>
-      <c r="E55" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
-        <v>199</v>
-      </c>
-      <c r="E56" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>200</v>
+        <v>198</v>
+      </c>
+      <c r="E57" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+      <c r="C64" t="s">
         <v>206</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D64" t="s">
+        <v>209</v>
+      </c>
+      <c r="E64" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
         <v>207</v>
       </c>
-      <c r="D63" t="s">
-        <v>210</v>
-      </c>
-      <c r="E63" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+      <c r="D66" t="s">
+        <v>143</v>
+      </c>
+      <c r="E66" t="s">
         <v>208</v>
       </c>
-      <c r="D65" t="s">
-        <v>144</v>
-      </c>
-      <c r="E65" t="s">
-        <v>209</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:D52 E4 E22 E25:E27 C55">
+  <conditionalFormatting sqref="E4 E22 E25:E27 C56 C3:D53">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Mean bar by gender/grade - 1var"</formula>
     </cfRule>

</xml_diff>